<commit_message>
begun grading HMWK 2
</commit_message>
<xml_diff>
--- a/Grades/GradeBook.xlsx
+++ b/Grades/GradeBook.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t xml:space="preserve">First name</t>
   </si>
@@ -34,6 +34,9 @@
     <t xml:space="preserve">Homework 1</t>
   </si>
   <si>
+    <t xml:space="preserve">Homework 2</t>
+  </si>
+  <si>
     <t xml:space="preserve">Gary</t>
   </si>
   <si>
@@ -50,6 +53,9 @@
   </si>
   <si>
     <t xml:space="preserve">jwarlum@poets.whittier.edu</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t xml:space="preserve">Aman</t>
@@ -259,17 +265,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.51953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.79"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -285,46 +292,56 @@
       <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" s="0" t="n">
         <f aca="false">35/35</f>
         <v>1</v>
       </c>
+      <c r="E2" s="0" t="n">
+        <f aca="false">26/25</f>
+        <v>1.04</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" s="0" t="n">
         <f aca="false">30/35</f>
         <v>0.857142857142857</v>
       </c>
+      <c r="E3" s="0" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D4" s="0" t="n">
         <f aca="false">35/35</f>
@@ -333,13 +350,13 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D5" s="0" t="n">
         <f aca="false">0</f>
@@ -348,13 +365,13 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D6" s="0" t="n">
         <f aca="false">0</f>
@@ -363,58 +380,69 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D7" s="0" t="n">
         <f aca="false">25/35</f>
         <v>0.714285714285714</v>
       </c>
+      <c r="E7" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D8" s="0" t="n">
         <f aca="false">35/35</f>
         <v>1</v>
       </c>
+      <c r="E8" s="0" t="n">
+        <f aca="false">20/25</f>
+        <v>0.8</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D9" s="0" t="n">
         <f aca="false">30/35</f>
         <v>0.857142857142857</v>
       </c>
+      <c r="E9" s="0" t="n">
+        <f aca="false">22/25</f>
+        <v>0.88</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D10" s="0" t="n">
         <f aca="false">35/35</f>
@@ -423,13 +451,13 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D11" s="0" t="n">
         <f aca="false">0</f>
@@ -438,13 +466,13 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D12" s="0" t="n">
         <f aca="false">0</f>
@@ -453,28 +481,32 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D13" s="0" t="n">
         <f aca="false">35/35</f>
         <v>1</v>
       </c>
+      <c r="E13" s="0" t="n">
+        <f aca="false">25/25</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D14" s="0" t="n">
         <f aca="false">30/35</f>
@@ -483,17 +515,21 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D15" s="0" t="n">
         <f aca="false">30/35</f>
         <v>0.857142857142857</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <f aca="false">17/25</f>
+        <v>0.68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added quiz 1 results
</commit_message>
<xml_diff>
--- a/Grades/GradeBook.xlsx
+++ b/Grades/GradeBook.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t xml:space="preserve">First name</t>
   </si>
@@ -37,6 +37,12 @@
     <t xml:space="preserve">Homework 2</t>
   </si>
   <si>
+    <t xml:space="preserve">Homework 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quiz 1</t>
+  </si>
+  <si>
     <t xml:space="preserve">Gary</t>
   </si>
   <si>
@@ -53,9 +59,6 @@
   </si>
   <si>
     <t xml:space="preserve">jwarlum@poets.whittier.edu</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t xml:space="preserve">Aman</t>
@@ -265,18 +268,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.51953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.53125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -295,16 +300,22 @@
       <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D2" s="0" t="n">
         <f aca="false">35/35</f>
@@ -314,97 +325,156 @@
         <f aca="false">26/25</f>
         <v>1.04</v>
       </c>
+      <c r="F2" s="0" t="n">
+        <f aca="false">29/30</f>
+        <v>0.966666666666667</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <f aca="false">55/50</f>
+        <v>1.1</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D3" s="0" t="n">
         <f aca="false">30/35</f>
         <v>0.857142857142857</v>
       </c>
-      <c r="E3" s="0" t="s">
-        <v>11</v>
+      <c r="E3" s="0" t="n">
+        <f aca="false">24/25</f>
+        <v>0.96</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <f aca="false">29/30</f>
+        <v>0.966666666666667</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <f aca="false">44/50</f>
+        <v>0.88</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D4" s="0" t="n">
         <f aca="false">35/35</f>
         <v>1</v>
       </c>
+      <c r="E4" s="0" t="n">
+        <f aca="false">27/25</f>
+        <v>1.08</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <f aca="false">30/30</f>
+        <v>1</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <f aca="false">55/50</f>
+        <v>1.1</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D5" s="0" t="n">
         <f aca="false">0</f>
         <v>0</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <f aca="false">25/25</f>
+        <v>1</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <f aca="false">29/30</f>
+        <v>0.966666666666667</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <f aca="false">55/50</f>
+        <v>1.1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D6" s="0" t="n">
         <f aca="false">0</f>
         <v>0</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <f aca="false">47/50</f>
+        <v>0.94</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D7" s="0" t="n">
         <f aca="false">25/35</f>
         <v>0.714285714285714</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>0</v>
+        <f aca="false">15/25</f>
+        <v>0.6</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <f aca="false">41/50</f>
+        <v>0.82</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D8" s="0" t="n">
         <f aca="false">35/35</f>
@@ -414,16 +484,24 @@
         <f aca="false">20/25</f>
         <v>0.8</v>
       </c>
+      <c r="F8" s="0" t="n">
+        <f aca="false">29/30</f>
+        <v>0.966666666666667</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <f aca="false">50/50</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D9" s="0" t="n">
         <f aca="false">30/35</f>
@@ -433,61 +511,102 @@
         <f aca="false">22/25</f>
         <v>0.88</v>
       </c>
+      <c r="F9" s="0" t="n">
+        <f aca="false">28/30</f>
+        <v>0.933333333333333</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <f aca="false">44/50</f>
+        <v>0.88</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D10" s="0" t="n">
         <f aca="false">35/35</f>
         <v>1</v>
       </c>
+      <c r="E10" s="0" t="n">
+        <f aca="false">25/25</f>
+        <v>1</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <f aca="false">29/30</f>
+        <v>0.966666666666667</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <f aca="false">55/50</f>
+        <v>1.1</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D11" s="0" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" s="0" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D12" s="0" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" s="0" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D13" s="0" t="n">
         <f aca="false">35/35</f>
@@ -497,31 +616,51 @@
         <f aca="false">25/25</f>
         <v>1</v>
       </c>
+      <c r="F13" s="0" t="n">
+        <f aca="false">29/30</f>
+        <v>0.966666666666667</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <f aca="false">47/50</f>
+        <v>0.94</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D14" s="0" t="n">
         <f aca="false">30/35</f>
         <v>0.857142857142857</v>
       </c>
+      <c r="E14" s="0" t="n">
+        <f aca="false">18/25</f>
+        <v>0.72</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <f aca="false">29/30</f>
+        <v>0.966666666666667</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <f aca="false">38/50</f>
+        <v>0.76</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D15" s="0" t="n">
         <f aca="false">30/35</f>
@@ -530,6 +669,14 @@
       <c r="E15" s="0" t="n">
         <f aca="false">17/25</f>
         <v>0.68</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <f aca="false">5/30</f>
+        <v>0.166666666666667</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added grades, warm ups, modified syllabus
</commit_message>
<xml_diff>
--- a/Grades/GradeBook.xlsx
+++ b/Grades/GradeBook.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t xml:space="preserve">First name</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t xml:space="preserve">Quiz 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Homework 4</t>
   </si>
   <si>
     <t xml:space="preserve">Gary</t>
@@ -268,13 +271,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
+      <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.53125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.41"/>
@@ -282,6 +285,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.89"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -306,16 +310,19 @@
       <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" s="0" t="n">
         <f aca="false">35/35</f>
@@ -333,16 +340,20 @@
         <f aca="false">55/50</f>
         <v>1.1</v>
       </c>
+      <c r="H2" s="0" t="n">
+        <f aca="false">19/20</f>
+        <v>0.95</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3" s="0" t="n">
         <f aca="false">30/35</f>
@@ -360,16 +371,20 @@
         <f aca="false">44/50</f>
         <v>0.88</v>
       </c>
+      <c r="H3" s="0" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D4" s="0" t="n">
         <f aca="false">35/35</f>
@@ -387,16 +402,20 @@
         <f aca="false">55/50</f>
         <v>1.1</v>
       </c>
+      <c r="H4" s="0" t="n">
+        <f aca="false">18/20</f>
+        <v>0.9</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D5" s="0" t="n">
         <f aca="false">0</f>
@@ -414,16 +433,20 @@
         <f aca="false">55/50</f>
         <v>1.1</v>
       </c>
+      <c r="H5" s="0" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D6" s="0" t="n">
         <f aca="false">0</f>
@@ -439,16 +462,20 @@
         <f aca="false">47/50</f>
         <v>0.94</v>
       </c>
+      <c r="H6" s="0" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D7" s="0" t="n">
         <f aca="false">25/35</f>
@@ -465,16 +492,20 @@
         <f aca="false">41/50</f>
         <v>0.82</v>
       </c>
+      <c r="H7" s="0" t="n">
+        <f aca="false">16/20</f>
+        <v>0.8</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D8" s="0" t="n">
         <f aca="false">35/35</f>
@@ -492,16 +523,20 @@
         <f aca="false">50/50</f>
         <v>1</v>
       </c>
+      <c r="H8" s="0" t="n">
+        <f aca="false">19/20</f>
+        <v>0.95</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D9" s="0" t="n">
         <f aca="false">30/35</f>
@@ -519,16 +554,20 @@
         <f aca="false">44/50</f>
         <v>0.88</v>
       </c>
+      <c r="H9" s="0" t="n">
+        <f aca="false">19/20</f>
+        <v>0.95</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D10" s="0" t="n">
         <f aca="false">35/35</f>
@@ -546,16 +585,20 @@
         <f aca="false">55/50</f>
         <v>1.1</v>
       </c>
+      <c r="H10" s="0" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D11" s="0" t="n">
         <f aca="false">0</f>
@@ -571,17 +614,21 @@
       <c r="G11" s="0" t="n">
         <f aca="false">0</f>
         <v>0</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <f aca="false">16/20</f>
+        <v>0.8</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D12" s="0" t="n">
         <f aca="false">0</f>
@@ -594,19 +641,23 @@
         <v>0</v>
       </c>
       <c r="G12" s="0" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="H12" s="0" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D13" s="0" t="n">
         <f aca="false">35/35</f>
@@ -624,16 +675,20 @@
         <f aca="false">47/50</f>
         <v>0.94</v>
       </c>
+      <c r="H13" s="0" t="n">
+        <f aca="false">16/20</f>
+        <v>0.8</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D14" s="0" t="n">
         <f aca="false">30/35</f>
@@ -651,16 +706,20 @@
         <f aca="false">38/50</f>
         <v>0.76</v>
       </c>
+      <c r="H14" s="0" t="n">
+        <f aca="false">17/20</f>
+        <v>0.85</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D15" s="0" t="n">
         <f aca="false">30/35</f>
@@ -677,6 +736,10 @@
       <c r="G15" s="0" t="n">
         <f aca="false">0</f>
         <v>0</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <f aca="false">5/20</f>
+        <v>0.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
grading update, midterm 2, code labs
</commit_message>
<xml_diff>
--- a/Grades/GradeBook.xlsx
+++ b/Grades/GradeBook.xlsx
@@ -274,10 +274,10 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
+      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.41"/>
@@ -730,16 +730,16 @@
         <v>0.68</v>
       </c>
       <c r="F15" s="0" t="n">
-        <f aca="false">5/30</f>
-        <v>0.166666666666667</v>
+        <f aca="false">28/30</f>
+        <v>0.933333333333333</v>
       </c>
       <c r="G15" s="0" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
+        <f aca="false">50/50</f>
+        <v>1</v>
       </c>
       <c r="H15" s="0" t="n">
-        <f aca="false">5/20</f>
-        <v>0.25</v>
+        <f aca="false">20/20</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
grading update, new warm up
</commit_message>
<xml_diff>
--- a/Grades/GradeBook.xlsx
+++ b/Grades/GradeBook.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t xml:space="preserve">First name</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t xml:space="preserve">Homework 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Homework 5</t>
   </si>
   <si>
     <t xml:space="preserve">Gary</t>
@@ -271,13 +274,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
+      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.41"/>
@@ -286,6 +289,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.99"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -313,16 +317,19 @@
       <c r="H1" s="0" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" s="0" t="n">
         <f aca="false">35/35</f>
@@ -344,16 +351,20 @@
         <f aca="false">19/20</f>
         <v>0.95</v>
       </c>
+      <c r="I2" s="0" t="n">
+        <f aca="false">25/25</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D3" s="0" t="n">
         <f aca="false">30/35</f>
@@ -375,16 +386,20 @@
         <f aca="false">0</f>
         <v>0</v>
       </c>
+      <c r="I3" s="0" t="n">
+        <f aca="false">25/25</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D4" s="0" t="n">
         <f aca="false">35/35</f>
@@ -406,20 +421,24 @@
         <f aca="false">18/20</f>
         <v>0.9</v>
       </c>
+      <c r="I4" s="0" t="n">
+        <f aca="false">25/25</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D5" s="0" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
+        <f aca="false">35/35</f>
+        <v>1</v>
       </c>
       <c r="E5" s="0" t="n">
         <f aca="false">25/25</f>
@@ -437,16 +456,20 @@
         <f aca="false">0</f>
         <v>0</v>
       </c>
+      <c r="I5" s="0" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D6" s="0" t="n">
         <f aca="false">0</f>
@@ -466,16 +489,20 @@
         <f aca="false">0</f>
         <v>0</v>
       </c>
+      <c r="I6" s="0" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D7" s="0" t="n">
         <f aca="false">25/35</f>
@@ -486,7 +513,8 @@
         <v>0.6</v>
       </c>
       <c r="F7" s="0" t="n">
-        <v>0</v>
+        <f aca="false">29/30</f>
+        <v>0.966666666666667</v>
       </c>
       <c r="G7" s="0" t="n">
         <f aca="false">41/50</f>
@@ -496,16 +524,20 @@
         <f aca="false">16/20</f>
         <v>0.8</v>
       </c>
+      <c r="I7" s="0" t="n">
+        <f aca="false">20/25</f>
+        <v>0.8</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D8" s="0" t="n">
         <f aca="false">35/35</f>
@@ -527,16 +559,20 @@
         <f aca="false">19/20</f>
         <v>0.95</v>
       </c>
+      <c r="I8" s="0" t="n">
+        <f aca="false">25/25</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D9" s="0" t="n">
         <f aca="false">30/35</f>
@@ -558,16 +594,20 @@
         <f aca="false">19/20</f>
         <v>0.95</v>
       </c>
+      <c r="I9" s="0" t="n">
+        <f aca="false">20/25</f>
+        <v>0.8</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D10" s="0" t="n">
         <f aca="false">35/35</f>
@@ -589,27 +629,32 @@
         <f aca="false">0</f>
         <v>0</v>
       </c>
+      <c r="I10" s="0" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D11" s="0" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
+        <f aca="false">30/35</f>
+        <v>0.857142857142857</v>
       </c>
       <c r="E11" s="0" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
+        <f aca="false">21/25</f>
+        <v>0.84</v>
       </c>
       <c r="F11" s="0" t="n">
-        <v>0</v>
+        <f aca="false">22/30</f>
+        <v>0.733333333333333</v>
       </c>
       <c r="G11" s="0" t="n">
         <f aca="false">0</f>
@@ -619,16 +664,20 @@
         <f aca="false">16/20</f>
         <v>0.8</v>
       </c>
+      <c r="I11" s="0" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D12" s="0" t="n">
         <f aca="false">0</f>
@@ -645,19 +694,23 @@
         <v>0</v>
       </c>
       <c r="H12" s="0" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="I12" s="0" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D13" s="0" t="n">
         <f aca="false">35/35</f>
@@ -679,16 +732,20 @@
         <f aca="false">16/20</f>
         <v>0.8</v>
       </c>
+      <c r="I13" s="0" t="n">
+        <f aca="false">25/25</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D14" s="0" t="n">
         <f aca="false">30/35</f>
@@ -710,16 +767,20 @@
         <f aca="false">17/20</f>
         <v>0.85</v>
       </c>
+      <c r="I14" s="0" t="n">
+        <f aca="false">25/25</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D15" s="0" t="n">
         <f aca="false">30/35</f>
@@ -739,6 +800,10 @@
       </c>
       <c r="H15" s="0" t="n">
         <f aca="false">20/20</f>
+        <v>1</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <f aca="false">25/25</f>
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
grading quiz 2, updated warm ups
</commit_message>
<xml_diff>
--- a/Grades/GradeBook.xlsx
+++ b/Grades/GradeBook.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t xml:space="preserve">First name</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t xml:space="preserve">Homework 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quiz 2</t>
   </si>
   <si>
     <t xml:space="preserve">Gary</t>
@@ -274,13 +277,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
+      <selection pane="topLeft" activeCell="J10" activeCellId="0" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.41"/>
@@ -320,16 +323,19 @@
       <c r="I1" s="0" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2" s="0" t="n">
         <f aca="false">35/35</f>
@@ -355,16 +361,20 @@
         <f aca="false">25/25</f>
         <v>1</v>
       </c>
+      <c r="J2" s="0" t="n">
+        <f aca="false">37/35</f>
+        <v>1.05714285714286</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D3" s="0" t="n">
         <f aca="false">30/35</f>
@@ -390,16 +400,20 @@
         <f aca="false">25/25</f>
         <v>1</v>
       </c>
+      <c r="J3" s="0" t="n">
+        <f aca="false">34/35</f>
+        <v>0.971428571428571</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D4" s="0" t="n">
         <f aca="false">35/35</f>
@@ -425,16 +439,20 @@
         <f aca="false">25/25</f>
         <v>1</v>
       </c>
+      <c r="J4" s="0" t="n">
+        <f aca="false">38/35</f>
+        <v>1.08571428571429</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D5" s="0" t="n">
         <f aca="false">35/35</f>
@@ -463,13 +481,13 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D6" s="0" t="n">
         <f aca="false">0</f>
@@ -496,13 +514,13 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D7" s="0" t="n">
         <f aca="false">25/35</f>
@@ -528,16 +546,20 @@
         <f aca="false">20/25</f>
         <v>0.8</v>
       </c>
+      <c r="J7" s="0" t="n">
+        <f aca="false">22/35</f>
+        <v>0.628571428571429</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D8" s="0" t="n">
         <f aca="false">35/35</f>
@@ -563,16 +585,20 @@
         <f aca="false">25/25</f>
         <v>1</v>
       </c>
+      <c r="J8" s="0" t="n">
+        <f aca="false">35/35</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D9" s="0" t="n">
         <f aca="false">30/35</f>
@@ -598,16 +624,20 @@
         <f aca="false">20/25</f>
         <v>0.8</v>
       </c>
+      <c r="J9" s="0" t="n">
+        <f aca="false">38/35</f>
+        <v>1.08571428571429</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D10" s="0" t="n">
         <f aca="false">35/35</f>
@@ -636,13 +666,13 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D11" s="0" t="n">
         <f aca="false">30/35</f>
@@ -671,13 +701,13 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D12" s="0" t="n">
         <f aca="false">0</f>
@@ -704,13 +734,13 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D13" s="0" t="n">
         <f aca="false">35/35</f>
@@ -736,16 +766,20 @@
         <f aca="false">25/25</f>
         <v>1</v>
       </c>
+      <c r="J13" s="0" t="n">
+        <f aca="false">31/35</f>
+        <v>0.885714285714286</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D14" s="0" t="n">
         <f aca="false">30/35</f>
@@ -771,16 +805,20 @@
         <f aca="false">25/25</f>
         <v>1</v>
       </c>
+      <c r="J14" s="0" t="n">
+        <f aca="false">34/35</f>
+        <v>0.971428571428571</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D15" s="0" t="n">
         <f aca="false">30/35</f>
@@ -805,6 +843,10 @@
       <c r="I15" s="0" t="n">
         <f aca="false">25/25</f>
         <v>1</v>
+      </c>
+      <c r="J15" s="0" t="n">
+        <f aca="false">37/35</f>
+        <v>1.05714285714286</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
grade update - PBL review
</commit_message>
<xml_diff>
--- a/Grades/GradeBook.xlsx
+++ b/Grades/GradeBook.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t xml:space="preserve">First name</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t xml:space="preserve">PBL Env</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raw Grade</t>
   </si>
   <si>
     <t xml:space="preserve">Gary</t>
@@ -283,13 +286,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.41"/>
@@ -299,6 +302,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="12.3"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -338,16 +342,19 @@
       <c r="L1" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="M1" s="0" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D2" s="0" t="n">
         <f aca="false">35/35</f>
@@ -377,16 +384,24 @@
         <f aca="false">37/35</f>
         <v>1.05714285714286</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L2" s="0" t="n">
+        <f aca="false">0.15+0.1</f>
+        <v>0.25</v>
+      </c>
+      <c r="M2" s="0" t="n">
+        <f aca="false">AVERAGE(D2:F2,D2:I2)*0.25+0.15*G2+0.15*J2+0.15*K2+L2</f>
+        <v>0.825330687830688</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D3" s="0" t="n">
         <f aca="false">30/35</f>
@@ -416,16 +431,24 @@
         <f aca="false">34/35</f>
         <v>0.971428571428571</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L3" s="0" t="n">
+        <f aca="false">0.2+0.1</f>
+        <v>0.3</v>
+      </c>
+      <c r="M3" s="0" t="n">
+        <f aca="false">+0.15*G3+0.15*J3+0.15*K3+L3</f>
+        <v>0.577714285714286</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D4" s="0" t="n">
         <f aca="false">35/35</f>
@@ -455,16 +478,24 @@
         <f aca="false">38/35</f>
         <v>1.08571428571429</v>
       </c>
+      <c r="L4" s="0" t="n">
+        <f aca="false">0.2+0.1</f>
+        <v>0.3</v>
+      </c>
+      <c r="M4" s="0" t="n">
+        <f aca="false">+0.15*G4+0.15*J4+0.15*K4+L4</f>
+        <v>0.627857142857144</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D5" s="0" t="n">
         <f aca="false">35/35</f>
@@ -494,16 +525,24 @@
         <f aca="false">37/35</f>
         <v>1.05714285714286</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L5" s="0" t="n">
+        <f aca="false">0.1+0.2</f>
+        <v>0.3</v>
+      </c>
+      <c r="M5" s="0" t="n">
+        <f aca="false">+0.15*G5+0.15*J5+0.15*K5+L5</f>
+        <v>0.623571428571429</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D6" s="0" t="n">
         <f aca="false">0</f>
@@ -532,16 +571,24 @@
         <f aca="false">0</f>
         <v>0</v>
       </c>
+      <c r="L6" s="0" t="n">
+        <f aca="false">0.17+0.08</f>
+        <v>0.25</v>
+      </c>
+      <c r="M6" s="0" t="n">
+        <f aca="false">+0.15*G6+0.15*J6+0.15*K6+L6</f>
+        <v>0.391</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D7" s="0" t="n">
         <f aca="false">25/35</f>
@@ -571,16 +618,24 @@
         <f aca="false">25/35</f>
         <v>0.714285714285714</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L7" s="0" t="n">
+        <f aca="false">0.1+0.2</f>
+        <v>0.3</v>
+      </c>
+      <c r="M7" s="0" t="n">
+        <f aca="false">+0.15*G7+0.15*J7+0.15*K7+L7</f>
+        <v>0.530142857142857</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D8" s="0" t="n">
         <f aca="false">35/35</f>
@@ -610,16 +665,24 @@
         <f aca="false">35/35</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L8" s="0" t="n">
+        <f aca="false">0.2+0.1</f>
+        <v>0.3</v>
+      </c>
+      <c r="M8" s="0" t="n">
+        <f aca="false">+0.15*G8+0.15*J8+0.15*K8+L8</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D9" s="0" t="n">
         <f aca="false">30/35</f>
@@ -649,16 +712,24 @@
         <f aca="false">38/35</f>
         <v>1.08571428571429</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L9" s="0" t="n">
+        <f aca="false">0.2+0.1</f>
+        <v>0.3</v>
+      </c>
+      <c r="M9" s="0" t="n">
+        <f aca="false">+0.15*G9+0.15*J9+0.15*K9+L9</f>
+        <v>0.594857142857143</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D10" s="0" t="n">
         <f aca="false">35/35</f>
@@ -688,16 +759,24 @@
         <f aca="false">0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L10" s="0" t="n">
+        <f aca="false">0.2+0.1</f>
+        <v>0.3</v>
+      </c>
+      <c r="M10" s="0" t="n">
+        <f aca="false">+0.15*G10+0.15*J10+0.15*K10+L10</f>
+        <v>0.465</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D11" s="0" t="n">
         <f aca="false">30/35</f>
@@ -727,16 +806,24 @@
         <f aca="false">0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L11" s="0" t="n">
+        <f aca="false">0.2+0.1</f>
+        <v>0.3</v>
+      </c>
+      <c r="M11" s="0" t="n">
+        <f aca="false">+0.15*G11+0.15*J11+0.15*K11+L11</f>
+        <v>0.405</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D12" s="0" t="n">
         <f aca="false">0</f>
@@ -764,16 +851,24 @@
         <f aca="false">0</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L12" s="0" t="n">
+        <f aca="false">0.17+0.08</f>
+        <v>0.25</v>
+      </c>
+      <c r="M12" s="0" t="n">
+        <f aca="false">+0.15*G12+0.15*J12+0.15*K12+L12</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D13" s="0" t="n">
         <f aca="false">35/35</f>
@@ -803,16 +898,24 @@
         <f aca="false">31/35</f>
         <v>0.885714285714286</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L13" s="0" t="n">
+        <f aca="false">0.2+0.1</f>
+        <v>0.3</v>
+      </c>
+      <c r="M13" s="0" t="n">
+        <f aca="false">+0.15*G13+0.15*J13+0.15*K13+L13</f>
+        <v>0.573857142857143</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D14" s="0" t="n">
         <f aca="false">30/35</f>
@@ -842,16 +945,24 @@
         <f aca="false">34/35</f>
         <v>0.971428571428571</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L14" s="0" t="n">
+        <f aca="false">0.2+0.1</f>
+        <v>0.3</v>
+      </c>
+      <c r="M14" s="0" t="n">
+        <f aca="false">+0.15*G14+0.15*J14+0.15*K14+L14</f>
+        <v>0.559714285714286</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D15" s="0" t="n">
         <f aca="false">30/35</f>
@@ -880,6 +991,14 @@
       <c r="J15" s="0" t="n">
         <f aca="false">37/35</f>
         <v>1.05714285714286</v>
+      </c>
+      <c r="L15" s="0" t="n">
+        <f aca="false">0.2+0.1</f>
+        <v>0.3</v>
+      </c>
+      <c r="M15" s="0" t="n">
+        <f aca="false">+0.15*G15+0.15*J15+0.15*K15+L15</f>
+        <v>0.608571428571429</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
grade update: quiz 3 and old work
</commit_message>
<xml_diff>
--- a/Grades/GradeBook.xlsx
+++ b/Grades/GradeBook.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="62">
   <si>
     <t xml:space="preserve">First name</t>
   </si>
@@ -64,6 +64,9 @@
     <t xml:space="preserve">wCurve</t>
   </si>
   <si>
+    <t xml:space="preserve">Letter</t>
+  </si>
+  <si>
     <t xml:space="preserve">Gary</t>
   </si>
   <si>
@@ -73,6 +76,9 @@
     <t xml:space="preserve">che@poets.whittier.edu</t>
   </si>
   <si>
+    <t xml:space="preserve">A-</t>
+  </si>
+  <si>
     <t xml:space="preserve">Jayden</t>
   </si>
   <si>
@@ -109,6 +115,9 @@
     <t xml:space="preserve">omartine@poets.whittier.edu</t>
   </si>
   <si>
+    <t xml:space="preserve">F</t>
+  </si>
+  <si>
     <t xml:space="preserve">Kai</t>
   </si>
   <si>
@@ -118,9 +127,6 @@
     <t xml:space="preserve">kstephen@poets.whittier.edu</t>
   </si>
   <si>
-    <t xml:space="preserve">A-</t>
-  </si>
-  <si>
     <t xml:space="preserve">James</t>
   </si>
   <si>
@@ -148,6 +154,9 @@
     <t xml:space="preserve">lgrey@poets.whittier.edu</t>
   </si>
   <si>
+    <t xml:space="preserve">B</t>
+  </si>
+  <si>
     <t xml:space="preserve">Almas</t>
   </si>
   <si>
@@ -157,6 +166,9 @@
     <t xml:space="preserve">awaseem@poets.whittier.edu</t>
   </si>
   <si>
+    <t xml:space="preserve">B+</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ty</t>
   </si>
   <si>
@@ -164,6 +176,9 @@
   </si>
   <si>
     <t xml:space="preserve">tcarlson@poets.whittier.edu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INC</t>
   </si>
   <si>
     <t xml:space="preserve">Nailyn</t>
@@ -294,8 +309,8 @@
   </sheetPr>
   <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K14" activeCellId="0" sqref="K14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="69" zoomScaleNormal="69" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O11" activeCellId="0" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -354,16 +369,19 @@
       <c r="N1" s="0" t="s">
         <v>13</v>
       </c>
+      <c r="O1" s="0" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D2" s="0" t="n">
         <f aca="false">35/35</f>
@@ -393,28 +411,35 @@
         <f aca="false">37/35</f>
         <v>1.05714285714286</v>
       </c>
+      <c r="K2" s="0" t="n">
+        <f aca="false">30/30</f>
+        <v>1</v>
+      </c>
       <c r="L2" s="0" t="n">
         <f aca="false">0.15+0.1</f>
         <v>0.25</v>
       </c>
       <c r="M2" s="0" t="n">
         <f aca="false">+0.15*G2+0.15*J2+0.15*K2+L2+0.25*AVERAGE(D2:F2,D2:I2)</f>
-        <v>0.825330687830688</v>
+        <v>0.975330687830688</v>
       </c>
       <c r="N2" s="0" t="n">
         <f aca="false">M2+0.035</f>
-        <v>0.860330687830688</v>
+        <v>1.01033068783069</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D3" s="0" t="n">
         <f aca="false">30/35</f>
@@ -444,28 +469,35 @@
         <f aca="false">34/35</f>
         <v>0.971428571428571</v>
       </c>
+      <c r="K3" s="0" t="n">
+        <f aca="false">30/30</f>
+        <v>1</v>
+      </c>
       <c r="L3" s="0" t="n">
         <f aca="false">0.2+0.1</f>
         <v>0.3</v>
       </c>
       <c r="M3" s="0" t="n">
         <f aca="false">+0.15*G3+0.15*J3+0.15*K3+L3+0.25*AVERAGE(D3:F3,D3:I3)</f>
-        <v>0.784592592592592</v>
+        <v>0.934592592592592</v>
       </c>
       <c r="N3" s="0" t="n">
         <f aca="false">M3+0.035</f>
-        <v>0.819592592592593</v>
+        <v>0.969592592592592</v>
+      </c>
+      <c r="O3" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D4" s="0" t="n">
         <f aca="false">35/35</f>
@@ -495,28 +527,35 @@
         <f aca="false">38/35</f>
         <v>1.08571428571429</v>
       </c>
+      <c r="K4" s="0" t="n">
+        <f aca="false">29/30</f>
+        <v>0.966666666666667</v>
+      </c>
       <c r="L4" s="0" t="n">
         <f aca="false">0.2+0.1</f>
         <v>0.3</v>
       </c>
       <c r="M4" s="0" t="n">
         <f aca="false">+0.15*G4+0.15*J4+0.15*K4+L4+0.25*AVERAGE(D4:F4,D4:I4)</f>
-        <v>0.882301587301588</v>
+        <v>1.02730158730159</v>
       </c>
       <c r="N4" s="0" t="n">
         <f aca="false">M4+0.035</f>
-        <v>0.917301587301588</v>
+        <v>1.06230158730159</v>
+      </c>
+      <c r="O4" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D5" s="0" t="n">
         <f aca="false">35/35</f>
@@ -562,16 +601,19 @@
         <f aca="false">M5+0.035</f>
         <v>1.05449735449735</v>
       </c>
+      <c r="O5" s="0" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D6" s="0" t="n">
         <f aca="false">0</f>
@@ -600,6 +642,10 @@
         <f aca="false">0</f>
         <v>0</v>
       </c>
+      <c r="K6" s="0" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
       <c r="L6" s="0" t="n">
         <f aca="false">0.17+0.08</f>
         <v>0.25</v>
@@ -612,16 +658,19 @@
         <f aca="false">M6+0.035</f>
         <v>0.452111111111111</v>
       </c>
+      <c r="O6" s="0" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D7" s="0" t="n">
         <f aca="false">25/35</f>
@@ -668,18 +717,18 @@
         <v>0.899084656084656</v>
       </c>
       <c r="O7" s="0" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D8" s="0" t="n">
         <f aca="false">35/35</f>
@@ -709,28 +758,35 @@
         <f aca="false">35/35</f>
         <v>1</v>
       </c>
+      <c r="K8" s="0" t="n">
+        <f aca="false">27/30</f>
+        <v>0.9</v>
+      </c>
       <c r="L8" s="0" t="n">
         <f aca="false">0.2+0.1</f>
         <v>0.3</v>
       </c>
       <c r="M8" s="0" t="n">
         <f aca="false">+0.15*G8+0.15*J8+0.15*K8+L8+0.25*AVERAGE(D8:F8,D8:I8)</f>
-        <v>0.835648148148148</v>
+        <v>0.970648148148148</v>
       </c>
       <c r="N8" s="0" t="n">
         <f aca="false">M8+0.035</f>
-        <v>0.870648148148148</v>
+        <v>1.00564814814815</v>
+      </c>
+      <c r="O8" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D9" s="0" t="n">
         <f aca="false">30/35</f>
@@ -760,28 +816,35 @@
         <f aca="false">38/35</f>
         <v>1.08571428571429</v>
       </c>
+      <c r="K9" s="0" t="n">
+        <f aca="false">29/30</f>
+        <v>0.966666666666667</v>
+      </c>
       <c r="L9" s="0" t="n">
         <f aca="false">0.2+0.1</f>
         <v>0.3</v>
       </c>
       <c r="M9" s="0" t="n">
         <f aca="false">+0.15*G9+0.15*J9+0.15*K9+L9+0.25*AVERAGE(D9:F9,D9:I9)</f>
-        <v>0.816272486772487</v>
+        <v>0.961272486772487</v>
       </c>
       <c r="N9" s="0" t="n">
         <f aca="false">M9+0.035</f>
-        <v>0.851272486772487</v>
+        <v>0.996272486772487</v>
+      </c>
+      <c r="O9" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D10" s="0" t="n">
         <f aca="false">35/35</f>
@@ -811,28 +874,35 @@
         <f aca="false">0</f>
         <v>0</v>
       </c>
+      <c r="K10" s="0" t="n">
+        <f aca="false">30/30</f>
+        <v>1</v>
+      </c>
       <c r="L10" s="0" t="n">
         <f aca="false">0.2+0.1</f>
         <v>0.3</v>
       </c>
       <c r="M10" s="0" t="n">
         <f aca="false">+0.15*G10+0.15*J10+0.15*K10+L10+0.25*AVERAGE(D10:F10,D10:I10)</f>
-        <v>0.66037037037037</v>
+        <v>0.81037037037037</v>
       </c>
       <c r="N10" s="0" t="n">
         <f aca="false">M10+0.035</f>
-        <v>0.69537037037037</v>
+        <v>0.84537037037037</v>
+      </c>
+      <c r="O10" s="0" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D11" s="0" t="n">
         <f aca="false">30/35</f>
@@ -855,12 +925,16 @@
         <v>0.8</v>
       </c>
       <c r="I11" s="0" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
+        <f aca="false">15/25</f>
+        <v>0.6</v>
       </c>
       <c r="J11" s="0" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
+        <f aca="false">29/35</f>
+        <v>0.828571428571429</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <f aca="false">28/30</f>
+        <v>0.933333333333333</v>
       </c>
       <c r="L11" s="0" t="n">
         <f aca="false">0.2+0.1</f>
@@ -868,22 +942,25 @@
       </c>
       <c r="M11" s="0" t="n">
         <f aca="false">+0.15*G11+0.15*J11+0.15*K11+L11+0.25*AVERAGE(D11:F11,D11:I11)</f>
-        <v>0.581693121693122</v>
+        <v>0.862645502645503</v>
       </c>
       <c r="N11" s="0" t="n">
         <f aca="false">M11+0.035</f>
-        <v>0.616693121693122</v>
+        <v>0.897645502645502</v>
+      </c>
+      <c r="O11" s="0" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="D12" s="0" t="n">
         <f aca="false">0</f>
@@ -908,6 +985,10 @@
         <v>0</v>
       </c>
       <c r="J12" s="0" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="K12" s="0" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
@@ -923,16 +1004,19 @@
         <f aca="false">M12+0.035</f>
         <v>0.285</v>
       </c>
+      <c r="O12" s="0" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="D13" s="0" t="n">
         <f aca="false">35/35</f>
@@ -962,28 +1046,35 @@
         <f aca="false">31/35</f>
         <v>0.885714285714286</v>
       </c>
+      <c r="K13" s="0" t="n">
+        <f aca="false">26/30</f>
+        <v>0.866666666666667</v>
+      </c>
       <c r="L13" s="0" t="n">
         <f aca="false">0.2+0.1</f>
         <v>0.3</v>
       </c>
       <c r="M13" s="0" t="n">
         <f aca="false">+0.15*G13+0.15*J13+0.15*K13+L13+0.25*AVERAGE(D13:F13,D13:I13)</f>
-        <v>0.814783068783069</v>
+        <v>0.944783068783069</v>
       </c>
       <c r="N13" s="0" t="n">
         <f aca="false">M13+0.035</f>
-        <v>0.849783068783069</v>
+        <v>0.979783068783069</v>
+      </c>
+      <c r="O13" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="D14" s="0" t="n">
         <f aca="false">30/35</f>
@@ -1029,16 +1120,19 @@
         <f aca="false">M14+0.035</f>
         <v>0.932287037037037</v>
       </c>
+      <c r="O14" s="0" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="D15" s="0" t="n">
         <f aca="false">30/35</f>
@@ -1068,17 +1162,24 @@
         <f aca="false">37/35</f>
         <v>1.05714285714286</v>
       </c>
+      <c r="K15" s="0" t="n">
+        <f aca="false">32/30</f>
+        <v>1.06666666666667</v>
+      </c>
       <c r="L15" s="0" t="n">
         <f aca="false">0.2+0.1</f>
         <v>0.3</v>
       </c>
       <c r="M15" s="0" t="n">
         <f aca="false">+0.15*G15+0.15*J15+0.15*K15+L15+0.25*AVERAGE(D15:F15,D15:I15)</f>
-        <v>0.829153439153439</v>
+        <v>0.989153439153439</v>
       </c>
       <c r="N15" s="0" t="n">
         <f aca="false">M15+0.035</f>
-        <v>0.864153439153439</v>
+        <v>1.02415343915344</v>
+      </c>
+      <c r="O15" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
grade update - Loren Grey quiz 2
</commit_message>
<xml_diff>
--- a/Grades/GradeBook.xlsx
+++ b/Grades/GradeBook.xlsx
@@ -76,57 +76,60 @@
     <t xml:space="preserve">che@poets.whittier.edu</t>
   </si>
   <si>
+    <t xml:space="preserve">A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jayden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Warlum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jwarlum@poets.whittier.edu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kumpawat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">akumpawa@poets.whittier.edu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nahom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anteneh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nanteneh@poets.whittier.edu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oswen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Martinez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">omartine@poets.whittier.edu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stephens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kstephen@poets.whittier.edu</t>
+  </si>
+  <si>
     <t xml:space="preserve">A-</t>
   </si>
   <si>
-    <t xml:space="preserve">Jayden</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Warlum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jwarlum@poets.whittier.edu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aman</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kumpawat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">akumpawa@poets.whittier.edu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nahom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anteneh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nanteneh@poets.whittier.edu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oswen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Martinez</t>
-  </si>
-  <si>
-    <t xml:space="preserve">omartine@poets.whittier.edu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kai</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stephens</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kstephen@poets.whittier.edu</t>
-  </si>
-  <si>
     <t xml:space="preserve">James</t>
   </si>
   <si>
@@ -152,9 +155,6 @@
   </si>
   <si>
     <t xml:space="preserve">lgrey@poets.whittier.edu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B</t>
   </si>
   <si>
     <t xml:space="preserve">Almas</t>
@@ -310,7 +310,7 @@
   <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="69" zoomScaleNormal="69" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O11" activeCellId="0" sqref="O11"/>
+      <selection pane="topLeft" activeCell="J6" activeCellId="0" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -717,18 +717,18 @@
         <v>0.899084656084656</v>
       </c>
       <c r="O7" s="0" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D8" s="0" t="n">
         <f aca="false">35/35</f>
@@ -780,13 +780,13 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D9" s="0" t="n">
         <f aca="false">30/35</f>
@@ -838,13 +838,13 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D10" s="0" t="n">
         <f aca="false">35/35</f>
@@ -871,8 +871,8 @@
         <v>0</v>
       </c>
       <c r="J10" s="0" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
+        <f aca="false">33/35</f>
+        <v>0.942857142857143</v>
       </c>
       <c r="K10" s="0" t="n">
         <f aca="false">30/30</f>
@@ -884,14 +884,14 @@
       </c>
       <c r="M10" s="0" t="n">
         <f aca="false">+0.15*G10+0.15*J10+0.15*K10+L10+0.25*AVERAGE(D10:F10,D10:I10)</f>
-        <v>0.81037037037037</v>
+        <v>0.951798941798942</v>
       </c>
       <c r="N10" s="0" t="n">
         <f aca="false">M10+0.035</f>
-        <v>0.84537037037037</v>
+        <v>0.986798941798942</v>
       </c>
       <c r="O10" s="0" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>